<commit_message>
Add sorting to unmatched items list
</commit_message>
<xml_diff>
--- a/database/Comparisons/po.xlsx
+++ b/database/Comparisons/po.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kurtm\Documents\GitHub\PerformanceHub\database\Comparisons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4741D7DE-F9B1-41D7-9EE4-691542810550}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{47407C4A-FE05-46D3-BFCC-E33F31FE56A2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" tabRatio="321" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12669" uniqueCount="1749">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12670" uniqueCount="1750">
   <si>
     <t>PO_Number</t>
   </si>
@@ -5357,6 +5357,9 @@
   </si>
   <si>
     <t>CSW-00NSB0S_STD~3/4X1/2</t>
+  </si>
+  <si>
+    <t>316W-AASMBB0_10S~3/4</t>
   </si>
 </sst>
 </file>
@@ -5542,7 +5545,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5733,20 +5736,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -6024,8 +6030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M1667"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D1688" sqref="D1688"/>
+    <sheetView tabSelected="1" topLeftCell="D22" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -19496,7 +19502,7 @@
       <c r="D347" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="E347" s="58">
+      <c r="E347" s="64">
         <v>72</v>
       </c>
       <c r="F347" s="59" t="s">
@@ -19535,7 +19541,7 @@
       <c r="D348" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="E348" s="58">
+      <c r="E348" s="64">
         <v>73</v>
       </c>
       <c r="F348" s="59" t="s">
@@ -19574,7 +19580,7 @@
       <c r="D349" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="E349" s="58">
+      <c r="E349" s="64">
         <v>74</v>
       </c>
       <c r="F349" s="59" t="s">
@@ -19613,7 +19619,7 @@
       <c r="D350" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="E350" s="58">
+      <c r="E350" s="64">
         <v>75</v>
       </c>
       <c r="F350" s="59" t="s">
@@ -19652,7 +19658,7 @@
       <c r="D351" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="E351" s="58">
+      <c r="E351" s="64">
         <v>76</v>
       </c>
       <c r="F351" s="59" t="s">
@@ -19691,7 +19697,7 @@
       <c r="D352" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="E352" s="58">
+      <c r="E352" s="64">
         <v>77</v>
       </c>
       <c r="F352" s="59" t="s">
@@ -19730,7 +19736,7 @@
       <c r="D353" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="E353" s="58">
+      <c r="E353" s="64">
         <v>78</v>
       </c>
       <c r="F353" s="59" t="s">
@@ -19769,7 +19775,7 @@
       <c r="D354" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="E354" s="58">
+      <c r="E354" s="64">
         <v>79</v>
       </c>
       <c r="F354" s="59" t="s">
@@ -19808,7 +19814,7 @@
       <c r="D355" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="E355" s="58">
+      <c r="E355" s="64">
         <v>80</v>
       </c>
       <c r="F355" s="59" t="s">
@@ -19847,7 +19853,7 @@
       <c r="D356" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="E356" s="58">
+      <c r="E356" s="64">
         <v>81</v>
       </c>
       <c r="F356" s="59" t="s">
@@ -19886,7 +19892,7 @@
       <c r="D357" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="E357" s="58">
+      <c r="E357" s="64">
         <v>82</v>
       </c>
       <c r="F357" s="59" t="s">
@@ -19925,7 +19931,7 @@
       <c r="D358" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="E358" s="58">
+      <c r="E358" s="64">
         <v>83</v>
       </c>
       <c r="F358" s="59" t="s">
@@ -19964,7 +19970,7 @@
       <c r="D359" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="E359" s="58">
+      <c r="E359" s="64">
         <v>84</v>
       </c>
       <c r="F359" s="59" t="s">
@@ -20003,7 +20009,7 @@
       <c r="D360" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="E360" s="58">
+      <c r="E360" s="64">
         <v>85</v>
       </c>
       <c r="F360" s="59" t="s">
@@ -20042,7 +20048,7 @@
       <c r="D361" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="E361" s="58">
+      <c r="E361" s="64">
         <v>86</v>
       </c>
       <c r="F361" s="59" t="s">
@@ -34936,7 +34942,7 @@
       <c r="D738" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E738" s="60">
+      <c r="E738" s="65">
         <v>59</v>
       </c>
       <c r="F738" s="60" t="s">
@@ -34977,7 +34983,7 @@
       <c r="D739" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E739" s="60">
+      <c r="E739" s="65">
         <v>60</v>
       </c>
       <c r="F739" s="60" t="s">
@@ -35018,7 +35024,7 @@
       <c r="D740" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E740" s="60">
+      <c r="E740" s="65">
         <v>61</v>
       </c>
       <c r="F740" s="60" t="s">
@@ -35059,7 +35065,7 @@
       <c r="D741" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E741" s="60">
+      <c r="E741" s="65">
         <v>62</v>
       </c>
       <c r="F741" s="60" t="s">
@@ -35100,7 +35106,7 @@
       <c r="D742" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E742" s="60">
+      <c r="E742" s="65">
         <v>63</v>
       </c>
       <c r="F742" s="60" t="s">
@@ -36043,7 +36049,7 @@
       <c r="D765" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E765" s="60">
+      <c r="E765" s="65">
         <v>86</v>
       </c>
       <c r="F765" s="60" t="s">
@@ -36084,7 +36090,7 @@
       <c r="D766" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E766" s="60">
+      <c r="E766" s="65">
         <v>87</v>
       </c>
       <c r="F766" s="60" t="s">
@@ -36125,7 +36131,7 @@
       <c r="D767" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E767" s="60">
+      <c r="E767" s="65">
         <v>88</v>
       </c>
       <c r="F767" s="60" t="s">
@@ -36166,7 +36172,7 @@
       <c r="D768" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E768" s="60">
+      <c r="E768" s="65">
         <v>89</v>
       </c>
       <c r="F768" s="60" t="s">
@@ -36207,7 +36213,7 @@
       <c r="D769" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E769" s="60">
+      <c r="E769" s="65">
         <v>90</v>
       </c>
       <c r="F769" s="60" t="s">
@@ -36248,7 +36254,7 @@
       <c r="D770" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E770" s="60">
+      <c r="E770" s="65">
         <v>91</v>
       </c>
       <c r="F770" s="60" t="s">
@@ -36289,7 +36295,7 @@
       <c r="D771" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E771" s="60">
+      <c r="E771" s="65">
         <v>92</v>
       </c>
       <c r="F771" s="60" t="s">
@@ -36330,7 +36336,7 @@
       <c r="D772" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E772" s="60">
+      <c r="E772" s="65">
         <v>93</v>
       </c>
       <c r="F772" s="60" t="s">
@@ -36371,7 +36377,7 @@
       <c r="D773" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E773" s="60">
+      <c r="E773" s="65">
         <v>94</v>
       </c>
       <c r="F773" s="60" t="s">
@@ -37215,7 +37221,9 @@
       <c r="L793" s="27">
         <v>0</v>
       </c>
-      <c r="M793" s="1"/>
+      <c r="M793" s="56" t="s">
+        <v>1749</v>
+      </c>
     </row>
     <row r="794" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A794" s="32" t="s">
@@ -49653,7 +49661,7 @@
       <c r="D1097" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="E1097" s="54">
+      <c r="E1097" s="66">
         <v>26</v>
       </c>
       <c r="F1097" s="54" t="s">
@@ -50063,7 +50071,7 @@
       <c r="D1107" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="E1107" s="54">
+      <c r="E1107" s="66">
         <v>36</v>
       </c>
       <c r="F1107" s="54" t="s">
@@ -50104,7 +50112,7 @@
       <c r="D1108" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="E1108" s="54">
+      <c r="E1108" s="66">
         <v>37</v>
       </c>
       <c r="F1108" s="54" t="s">
@@ -50145,7 +50153,7 @@
       <c r="D1109" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="E1109" s="54">
+      <c r="E1109" s="66">
         <v>38</v>
       </c>
       <c r="F1109" s="54" t="s">
@@ -50186,7 +50194,7 @@
       <c r="D1110" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="E1110" s="54">
+      <c r="E1110" s="66">
         <v>39</v>
       </c>
       <c r="F1110" s="54" t="s">
@@ -50227,7 +50235,7 @@
       <c r="D1111" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="E1111" s="54">
+      <c r="E1111" s="66">
         <v>40</v>
       </c>
       <c r="F1111" s="54" t="s">
@@ -50268,7 +50276,7 @@
       <c r="D1112" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="E1112" s="54">
+      <c r="E1112" s="66">
         <v>41</v>
       </c>
       <c r="F1112" s="54" t="s">
@@ -50309,7 +50317,7 @@
       <c r="D1113" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="E1113" s="54">
+      <c r="E1113" s="66">
         <v>42</v>
       </c>
       <c r="F1113" s="54" t="s">
@@ -50350,7 +50358,7 @@
       <c r="D1114" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="E1114" s="54">
+      <c r="E1114" s="66">
         <v>43</v>
       </c>
       <c r="F1114" s="54" t="s">
@@ -50391,7 +50399,7 @@
       <c r="D1115" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="E1115" s="54">
+      <c r="E1115" s="66">
         <v>44</v>
       </c>
       <c r="F1115" s="54" t="s">
@@ -69053,7 +69061,7 @@
       <c r="D1575" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E1575" s="63">
+      <c r="E1575" s="67">
         <v>41</v>
       </c>
       <c r="F1575" s="63" t="s">
@@ -69094,7 +69102,7 @@
       <c r="D1576" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E1576" s="63">
+      <c r="E1576" s="67">
         <v>42</v>
       </c>
       <c r="F1576" s="63" t="s">
@@ -69135,7 +69143,7 @@
       <c r="D1577" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E1577" s="63">
+      <c r="E1577" s="67">
         <v>43</v>
       </c>
       <c r="F1577" s="63" t="s">
@@ -69176,7 +69184,7 @@
       <c r="D1578" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="E1578" s="63">
+      <c r="E1578" s="67">
         <v>44</v>
       </c>
       <c r="F1578" s="63" t="s">

</xml_diff>